<commit_message>
Added unsatruated version of painting to denote non-interactivity. Split XML specifications into better defined chunks (seperated painting from hunt and menu from about) and updated HuntImporter accordingly.
</commit_message>
<xml_diff>
--- a/Painting Scavenger Hunt/xml/content parameters.xlsx
+++ b/Painting Scavenger Hunt/xml/content parameters.xlsx
@@ -17,29 +17,35 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="end goal" type="4" refreshedVersion="0" background="1">
+  <connection id="1" name="about" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\about.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" name="end goal" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\end goal.xml" htmlTables="1"/>
   </connection>
-  <connection id="2" name="hunt and painting" type="4" refreshedVersion="0" background="1">
+  <connection id="3" name="hunt and painting" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\hunt and painting.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="3" name="objects of interest" type="4" refreshedVersion="0" background="1">
+  <connection id="4" name="objects of interest" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\objects of interest.xml" htmlTables="1"/>
   </connection>
-  <connection id="4" name="painting" type="4" refreshedVersion="0" background="1">
+  <connection id="5" name="painting" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\painting.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="5" name="start-up" type="4" refreshedVersion="0" background="1">
+  <connection id="6" name="painting1" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\painting.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="7" name="start-up" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\start-up.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="6" name="start-up params" type="4" refreshedVersion="0" background="1">
+  <connection id="8" name="start-up params" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\Samuel E. Trapp\Desktop\tnbtb\nbtbquill\Painting Scavenger Hunt\xml\start-up params.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>title</t>
   </si>
@@ -518,10 +524,13 @@
     <t>obejcts of interest.xml</t>
   </si>
   <si>
-    <t>start-up.xml</t>
-  </si>
-  <si>
-    <t>hunt and painting.xml</t>
+    <t>assets/interface/NightBeforeTheBattle_HDR_Unsaturated.jpg</t>
+  </si>
+  <si>
+    <t>painting.xml</t>
+  </si>
+  <si>
+    <t>about.xml</t>
   </si>
 </sst>
 </file>
@@ -651,35 +660,25 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema4">
+  <Schema ID="Schema5">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Hunt">
+      <xsd:element nillable="true" name="Painting">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" name="Painting" form="unqualified">
-              <xsd:complexType>
-                <xsd:sequence minOccurs="0">
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="title" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="artist" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="interactive_filename" form="unqualified"/>
-                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="non-interactive_filename" form="unqualified"/>
-                </xsd:sequence>
-              </xsd:complexType>
-            </xsd:element>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="title" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="artist" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="interactive_filename" form="unqualified"/>
+            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="non-interactive_filename" form="unqualified"/>
           </xsd:sequence>
-          <xsd:attribute name="magnify_scale" form="unqualified" type="xsd:integer"/>
-          <xsd:attribute name="magnify_radius" form="unqualified" type="xsd:integer"/>
-          <xsd:attribute name="hunt_count" form="unqualified" type="xsd:integer"/>
         </xsd:complexType>
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Schema ID="Schema6">
+  <Schema ID="Schema7">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="Start-Up">
+      <xsd:element nillable="true" name="About">
         <xsd:complexType>
           <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="menu_color" form="unqualified"/>
             <xsd:element minOccurs="0" nillable="true" name="Splash_Screen" form="unqualified">
               <xsd:complexType>
                 <xsd:sequence minOccurs="0">
@@ -694,23 +693,23 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="3" Name="End_Goal_Map" RootElement="End_Goal" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="10" Name="About_Map" RootElement="About" SchemaID="Schema7" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="6" Name="Hunt_Map" RootElement="Hunt" SchemaID="Schema4" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="3" Name="End_Goal_Map" RootElement="End_Goal" SchemaID="Schema3" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
   <Map ID="2" Name="OOIs_Map" RootElement="OOIs" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="3" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="4" DataBindingLoadMode="1"/>
   </Map>
-  <Map ID="8" Name="Start-Up_Map" RootElement="Start-Up" SchemaID="Schema6" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="5" DataBindingLoadMode="1"/>
+  <Map ID="9" Name="Painting_Map" RootElement="Painting" SchemaID="Schema5" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="6" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:K32" tableType="xml" totalsRowShown="0" connectionId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A17:K32" tableType="xml" totalsRowShown="0" connectionId="4">
   <autoFilter ref="A17:K32"/>
   <tableColumns count="11">
     <tableColumn id="1" uniqueName="name" name="name">
@@ -752,7 +751,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A37:C45" tableType="xml" totalsRowShown="0" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A37:C45" tableType="xml" totalsRowShown="0" connectionId="2">
   <autoFilter ref="A37:C45"/>
   <tableColumns count="3">
     <tableColumn id="1" uniqueName="name" name="name">
@@ -771,39 +770,39 @@
 
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <singleXmlCell id="1" r="B2" connectionId="2">
+  <singleXmlCell id="1" r="B2" connectionId="6">
     <xmlCellPr id="1" uniqueName="title">
-      <xmlPr mapId="6" xpath="/Hunt/Painting/title" xmlDataType="string"/>
+      <xmlPr mapId="9" xpath="/Painting/title" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="2" r="B3" connectionId="2">
+  <singleXmlCell id="2" r="B3" connectionId="6">
     <xmlCellPr id="1" uniqueName="artist">
-      <xmlPr mapId="6" xpath="/Hunt/Painting/artist" xmlDataType="string"/>
+      <xmlPr mapId="9" xpath="/Painting/artist" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="3" r="B4" connectionId="2">
+  <singleXmlCell id="3" r="B4" connectionId="6">
     <xmlCellPr id="1" uniqueName="interactive_filename">
-      <xmlPr mapId="6" xpath="/Hunt/Painting/interactive_filename" xmlDataType="string"/>
+      <xmlPr mapId="9" xpath="/Painting/interactive_filename" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="4" r="B5" connectionId="2">
+  <singleXmlCell id="4" r="B5" connectionId="6">
     <xmlCellPr id="1" uniqueName="non-interactive_filename">
-      <xmlPr mapId="6" xpath="/Hunt/Painting/non-interactive_filename" xmlDataType="string"/>
+      <xmlPr mapId="9" xpath="/Painting/non-interactive_filename" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="14" r="B10" connectionId="5">
+  <singleXmlCell id="8" r="B10" connectionId="1">
     <xmlCellPr id="1" uniqueName="credits_text_file">
-      <xmlPr mapId="8" xpath="/Start-Up/Splash_Screen/credits_text_file" xmlDataType="string"/>
+      <xmlPr mapId="10" xpath="/About/Splash_Screen/credits_text_file" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="15" r="B11" connectionId="5">
+  <singleXmlCell id="9" r="B11" connectionId="1">
     <xmlCellPr id="1" uniqueName="about_text_file">
-      <xmlPr mapId="8" xpath="/Start-Up/Splash_Screen/about_text_file" xmlDataType="string"/>
+      <xmlPr mapId="10" xpath="/About/Splash_Screen/about_text_file" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="16" r="B12" connectionId="5">
+  <singleXmlCell id="10" r="B12" connectionId="1">
     <xmlCellPr id="1" uniqueName="tutorial_text_file">
-      <xmlPr mapId="8" xpath="/Start-Up/Splash_Screen/tutorial_text_file" xmlDataType="string"/>
+      <xmlPr mapId="10" xpath="/About/Splash_Screen/tutorial_text_file" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -1097,13 +1096,13 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="78" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
@@ -1155,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75">
@@ -1163,7 +1162,7 @@
         <v>150</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:2">

</xml_diff>

<commit_message>
TutorialMenu changed to InstructionsMenu. Ending no provides a new game option. Parrott rifle saturated color change. OOI highlights changed to be satruated images.
</commit_message>
<xml_diff>
--- a/Painting Scavenger Hunt/xml/content parameters.xlsx
+++ b/Painting Scavenger Hunt/xml/content parameters.xlsx
@@ -236,186 +236,6 @@
     <t>For most, selecting me should be part of your daily routine...</t>
   </si>
   <si>
-    <t>assets/ooi info/quill info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/moon info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/flag info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/skeleton info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/musket info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/silhouette info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/fire info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/cannonball info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/sword info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/cards info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/parrott rifle info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/sergeant info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/gabions info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/signature info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi info/uniform info.txt</t>
-  </si>
-  <si>
-    <t>assets/ooi images/quill hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/moon hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/flag hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/skeleton hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/musket hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/silhouette hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/fire hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cannonball hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sword hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cards hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/parrott rifle hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sergeant hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/gabions hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/signature hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/uniform hitmap.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/quill highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/moon highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/flag highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/skeleton highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/musket highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/silhouette highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/fire highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cannonball highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sword highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cards highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/parrott rifle highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sergeant highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/gabions highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/signature highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/uniform highlight.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/quill saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/moon saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/flag saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/skeleton saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/musket saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/silhouette saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/fire saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cannonball saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sword saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/cards saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/parrott rifle saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/sergeant saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/gabions saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/signature saturated.png</t>
-  </si>
-  <si>
-    <t>assets/ooi images/uniform saturated.png</t>
-  </si>
-  <si>
     <t>Objects of Interest</t>
   </si>
   <si>
@@ -534,6 +354,186 @@
   </si>
   <si>
     <t>non_interactive_filename</t>
+  </si>
+  <si>
+    <t>quill info.txt</t>
+  </si>
+  <si>
+    <t>moon info.txt</t>
+  </si>
+  <si>
+    <t>flag info.txt</t>
+  </si>
+  <si>
+    <t>skeleton info.txt</t>
+  </si>
+  <si>
+    <t>musket info.txt</t>
+  </si>
+  <si>
+    <t>silhouette info.txt</t>
+  </si>
+  <si>
+    <t>fire info.txt</t>
+  </si>
+  <si>
+    <t>cannonball info.txt</t>
+  </si>
+  <si>
+    <t>sword info.txt</t>
+  </si>
+  <si>
+    <t>cards info.txt</t>
+  </si>
+  <si>
+    <t>parrott rifle info.txt</t>
+  </si>
+  <si>
+    <t>sergeant info.txt</t>
+  </si>
+  <si>
+    <t>gabions info.txt</t>
+  </si>
+  <si>
+    <t>signature info.txt</t>
+  </si>
+  <si>
+    <t>uniform info.txt</t>
+  </si>
+  <si>
+    <t>quill hitmap.png</t>
+  </si>
+  <si>
+    <t>moon hitmap.png</t>
+  </si>
+  <si>
+    <t>flag hitmap.png</t>
+  </si>
+  <si>
+    <t>skeleton hitmap.png</t>
+  </si>
+  <si>
+    <t>musket hitmap.png</t>
+  </si>
+  <si>
+    <t>silhouette hitmap.png</t>
+  </si>
+  <si>
+    <t>fire hitmap.png</t>
+  </si>
+  <si>
+    <t>cannonball hitmap.png</t>
+  </si>
+  <si>
+    <t>sword hitmap.png</t>
+  </si>
+  <si>
+    <t>cards hitmap.png</t>
+  </si>
+  <si>
+    <t>parrott rifle hitmap.png</t>
+  </si>
+  <si>
+    <t>sergeant hitmap.png</t>
+  </si>
+  <si>
+    <t>gabions hitmap.png</t>
+  </si>
+  <si>
+    <t>signature hitmap.png</t>
+  </si>
+  <si>
+    <t>uniform hitmap.png</t>
+  </si>
+  <si>
+    <t>quill highlight.png</t>
+  </si>
+  <si>
+    <t>moon highlight.png</t>
+  </si>
+  <si>
+    <t>flag highlight.png</t>
+  </si>
+  <si>
+    <t>skeleton highlight.png</t>
+  </si>
+  <si>
+    <t>musket highlight.png</t>
+  </si>
+  <si>
+    <t>silhouette highlight.png</t>
+  </si>
+  <si>
+    <t>fire highlight.png</t>
+  </si>
+  <si>
+    <t>cannonball highlight.png</t>
+  </si>
+  <si>
+    <t>sword highlight.png</t>
+  </si>
+  <si>
+    <t>cards highlight.png</t>
+  </si>
+  <si>
+    <t>parrott rifle highlight.png</t>
+  </si>
+  <si>
+    <t>sergeant highlight.png</t>
+  </si>
+  <si>
+    <t>gabions highlight.png</t>
+  </si>
+  <si>
+    <t>signature highlight.png</t>
+  </si>
+  <si>
+    <t>uniform highlight.png</t>
+  </si>
+  <si>
+    <t>quill saturated.png</t>
+  </si>
+  <si>
+    <t>moon saturated.png</t>
+  </si>
+  <si>
+    <t>flag saturated.png</t>
+  </si>
+  <si>
+    <t>skeleton saturated.png</t>
+  </si>
+  <si>
+    <t>musket saturated.png</t>
+  </si>
+  <si>
+    <t>silhouette saturated.png</t>
+  </si>
+  <si>
+    <t>fire saturated.png</t>
+  </si>
+  <si>
+    <t>cannonball saturated.png</t>
+  </si>
+  <si>
+    <t>sword saturated.png</t>
+  </si>
+  <si>
+    <t>cards saturated.png</t>
+  </si>
+  <si>
+    <t>parrott rifle saturated.png</t>
+  </si>
+  <si>
+    <t>sergeant saturated.png</t>
+  </si>
+  <si>
+    <t>gabions saturated.png</t>
+  </si>
+  <si>
+    <t>signature saturated.png</t>
+  </si>
+  <si>
+    <t>uniform saturated.png</t>
   </si>
 </sst>
 </file>
@@ -1099,22 +1099,21 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="57" customWidth="1"/>
-    <col min="3" max="3" width="78" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="7" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" customWidth="1"/>
-    <col min="9" max="9" width="41.5703125" customWidth="1"/>
-    <col min="10" max="10" width="45.42578125" customWidth="1"/>
-    <col min="11" max="11" width="44" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="57.7109375" customWidth="1"/>
+    <col min="3" max="3" width="76.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
     <col min="12" max="12" width="39.5703125" customWidth="1"/>
     <col min="13" max="13" width="41.140625" customWidth="1"/>
     <col min="14" max="14" width="41.7109375" customWidth="1"/>
@@ -1122,10 +1121,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>159</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1154,50 +1153,50 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>149</v>
+        <v>89</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>160</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>150</v>
+        <v>90</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75">
       <c r="A16" s="1" t="s">
-        <v>122</v>
+        <v>62</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>157</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1246,13 +1245,13 @@
         <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>62</v>
+        <v>102</v>
       </c>
       <c r="E18">
         <v>0.78448269999999998</v>
       </c>
       <c r="F18">
-        <v>0.70186368635999996</v>
+        <v>0.70486368635999996</v>
       </c>
       <c r="G18">
         <v>0.35</v>
@@ -1261,13 +1260,13 @@
         <v>0.2</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>77</v>
+        <v>117</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1281,7 +1280,7 @@
         <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>103</v>
       </c>
       <c r="E19">
         <v>0.138931</v>
@@ -1296,13 +1295,13 @@
         <v>0.02</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1316,7 +1315,7 @@
         <v>49</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>104</v>
       </c>
       <c r="E20">
         <v>0.53965510000000005</v>
@@ -1331,13 +1330,13 @@
         <v>0.2</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>79</v>
+        <v>119</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>94</v>
+        <v>134</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1351,7 +1350,7 @@
         <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="E21">
         <v>0.45558270000000001</v>
@@ -1366,13 +1365,13 @@
         <v>0.1</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>95</v>
+        <v>135</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>110</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1386,7 +1385,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="E22">
         <v>0.62320679999999995</v>
@@ -1401,13 +1400,13 @@
         <v>0.2</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>81</v>
+        <v>121</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>96</v>
+        <v>136</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>111</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1421,7 +1420,7 @@
         <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>67</v>
+        <v>107</v>
       </c>
       <c r="E23">
         <v>0.87013790000000002</v>
@@ -1436,13 +1435,13 @@
         <v>0.02</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>82</v>
+        <v>122</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>97</v>
+        <v>137</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>112</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1456,7 +1455,7 @@
         <v>53</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="E24">
         <v>0.1772068</v>
@@ -1471,13 +1470,13 @@
         <v>0.2</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1491,7 +1490,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="E25">
         <v>6.0689600000000003E-2</v>
@@ -1506,13 +1505,13 @@
         <v>0.2</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>99</v>
+        <v>139</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1526,7 +1525,7 @@
         <v>55</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>70</v>
+        <v>110</v>
       </c>
       <c r="E26">
         <v>0.84855170000000002</v>
@@ -1541,13 +1540,13 @@
         <v>0.2</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1561,7 +1560,7 @@
         <v>56</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="E27">
         <v>0.39137929999999999</v>
@@ -1576,13 +1575,13 @@
         <v>0.2</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="K27" s="3" t="s">
-        <v>116</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1596,7 +1595,7 @@
         <v>57</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>72</v>
+        <v>112</v>
       </c>
       <c r="E28">
         <v>0.2560307</v>
@@ -1611,13 +1610,13 @@
         <v>0.1</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>102</v>
+        <v>142</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>117</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1631,7 +1630,7 @@
         <v>58</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>73</v>
+        <v>113</v>
       </c>
       <c r="E29">
         <v>0.48</v>
@@ -1646,13 +1645,13 @@
         <v>0.1</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>88</v>
+        <v>128</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="K29" s="3" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1666,7 +1665,7 @@
         <v>59</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="E30">
         <v>5.0000000000000001E-3</v>
@@ -1681,13 +1680,13 @@
         <v>0.1</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="J30" s="3" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1701,7 +1700,7 @@
         <v>60</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="E31">
         <v>6.0306999999999999E-3</v>
@@ -1716,13 +1715,13 @@
         <v>0.15</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="J31" s="3" t="s">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1736,7 +1735,7 @@
         <v>61</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="E32">
         <v>0.29603069999999998</v>
@@ -1751,21 +1750,21 @@
         <v>0.2</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="J32" s="3" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="18.75">
       <c r="A36" s="1" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1773,7 +1772,7 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
@@ -1781,90 +1780,90 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>133</v>
+        <v>73</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>142</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>127</v>
+        <v>67</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>143</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>136</v>
+        <v>76</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>144</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>129</v>
+        <v>69</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>137</v>
+        <v>77</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>138</v>
+        <v>78</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>146</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>131</v>
+        <v>71</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>139</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>147</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>140</v>
+        <v>80</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>141</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>